<commit_message>
few code changes for data dictionary functionality
</commit_message>
<xml_diff>
--- a/Features/DataDictionary/userInputs/case_dd.xlsx
+++ b/Features/DataDictionary/userInputs/case_dd.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FL_LPT-567\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\GIT_Code\dimagi-qa\Features\DataDictionary\userInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC55453A-A398-4B54-8859-66D2B3C169C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3562D483-7066-47E1-A3C7-7B484FBFD645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="cases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>number</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>derfg</t>
+  </si>
+  <si>
+    <t>dd_4</t>
+  </si>
+  <si>
+    <t>uieyfhr</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>awerdfs</t>
   </si>
 </sst>
 </file>
@@ -420,16 +432,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" activeCellId="1" sqref="K5 C8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
   </cols>
@@ -488,7 +501,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -511,7 +524,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -523,12 +536,35 @@
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
       <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1">
+        <v>43864</v>
+      </c>
+      <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>